<commit_message>
commit april 20 changes
</commit_message>
<xml_diff>
--- a/_pslReport.xlsx
+++ b/_pslReport.xlsx
@@ -225,20 +225,20 @@
       <name val="Cambria"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
       <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
@@ -411,7 +411,61 @@
     <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -426,79 +480,25 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="9" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="4" numFmtId="9" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
@@ -551,7 +551,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
@@ -904,7 +904,7 @@
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="55" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="55" view="pageLayout" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
@@ -928,73 +928,73 @@
       <c r="M1"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="35"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="36" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="37"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="28"/>
     </row>
     <row r="11" spans="1:17" customHeight="1" ht="30">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="13" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="7" t="s">
@@ -1003,44 +1003,44 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="20" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="22"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="40"/>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="3"/>
@@ -1062,47 +1062,47 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" customHeight="1" ht="14.45">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28" t="s">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="38" t="s">
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="29" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:17" customHeight="1" ht="67.15">
-      <c r="A16" s="29"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1127,26 +1127,26 @@
       <c r="P16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="38"/>
+      <c r="Q16" s="29"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="41" t="s">
@@ -1260,23 +1260,23 @@
       <c r="Q20" s="41"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="43" t="s">
@@ -1320,289 +1320,289 @@
       <c r="Q22" s="44"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="39"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="39"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="39"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="39"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="39"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="39"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="39"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="39"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="39"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="39"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="39"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="39"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="39"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="4"/>
@@ -1797,6 +1797,25 @@
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E11:Q11"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="E12:Q12"/>
+    <mergeCell ref="E13:Q13"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="C15:D15"/>
@@ -1810,29 +1829,10 @@
     <mergeCell ref="Q15:Q16"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E11:Q11"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="E12:Q12"/>
-    <mergeCell ref="E13:Q13"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" scale="80" fitToHeight="0" fitToWidth="1"/>
+  <pageSetup paperSize="9" orientation="landscape" scale="76" fitToHeight="0" fitToWidth="1"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>